<commit_message>
cambios inicio dde semestre 2020 - 2
</commit_message>
<xml_diff>
--- a/HFC.xlsx
+++ b/HFC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanespejo/Documents/reveal/filociencia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836A6BD0-8CF0-1645-AA0C-52768AE5A0F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF6B832-08A6-2F4A-9830-6132468254B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{92AD9A07-1A21-864F-8FD9-98EB9AF3C646}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{92AD9A07-1A21-864F-8FD9-98EB9AF3C646}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="129">
   <si>
     <t>Viernes</t>
   </si>
@@ -71,21 +71,12 @@
     <t>Repaso</t>
   </si>
   <si>
-    <t>Problemas de la concepción heredada</t>
-  </si>
-  <si>
     <t>Quine: Dos dogmas del empirismo</t>
   </si>
   <si>
-    <t>Popper: contra la concepción heredada</t>
-  </si>
-  <si>
     <t>Popper: conjeturas y refutaciones</t>
   </si>
   <si>
-    <t>Semana santa</t>
-  </si>
-  <si>
     <t>AMAYA HERNANDEZ, JUAN ESTEBAN</t>
   </si>
   <si>
@@ -96,18 +87,6 @@
   </si>
   <si>
     <t>15%</t>
-  </si>
-  <si>
-    <t>Paradigmas científicos I</t>
-  </si>
-  <si>
-    <t>Paradigmas científicos II</t>
-  </si>
-  <si>
-    <t>La concepción heredada de las teorías científicas I</t>
-  </si>
-  <si>
-    <t>La concepción heredada de las teorías científicas II</t>
   </si>
   <si>
     <t>Vnum</t>
@@ -167,9 +146,6 @@
     </r>
   </si>
   <si>
-    <t>(*) Fine, A. (1986). The Shaky Game.  Chicago, USA: The University of Chicago Press. Caps 1, 3 y 5 (★)</t>
-  </si>
-  <si>
     <r>
       <t>Suppe, Frederick (1979) </t>
     </r>
@@ -192,66 +168,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Quine, W. V. O. (2002) Desde un punto de vista lógico. Paidos: Barcelona, España. Capítulo 2 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="28"/>
-        <color rgb="FFEAEAEA"/>
-        <rFont val="PingFang SC"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>★</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="28"/>
-        <color rgb="FFEAEAEA"/>
-        <rFont val="Helvetica"/>
-        <family val="2"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Popper, K (2002) </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Inherit"/>
-      </rPr>
-      <t>Conjeturas y refutaciones. Paidos: Barcelona, España. Capítulo 1 (★)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Kuhn, Thomas (1962) </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Inherit"/>
-      </rPr>
-      <t>La estructura de las revoluciones científicas</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Inherit"/>
-      </rPr>
-      <t>. Fondo de cultura económica: México. Capítulos 1, 2 (★), 3 (★), 4, 5 (★) y 6 (★)</t>
-    </r>
-  </si>
-  <si>
     <t>Estudiantes</t>
   </si>
   <si>
@@ -483,25 +399,7 @@
     <t>¡Todo!</t>
   </si>
   <si>
-    <t>Nada</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> el examen final en virtual sabana</t>
-  </si>
-  <si>
-    <t>Examen primer corte</t>
-  </si>
-  <si>
-    <t>Examen segundo corte</t>
-  </si>
-  <si>
-    <t>Examen tercer corte</t>
-  </si>
-  <si>
     <t>el taller en virtual sabana</t>
-  </si>
-  <si>
-    <t>Lunes</t>
   </si>
   <si>
     <t>Los inicios del método axiomático y la explicación aristotélica</t>
@@ -544,7 +442,51 @@
     </r>
   </si>
   <si>
-    <t>Licencia de paternidad :)</t>
+    <t>Ciencia y valores: Filosofía feminista de la ciencia</t>
+  </si>
+  <si>
+    <t>Martes</t>
+  </si>
+  <si>
+    <t>Empirismo lógico</t>
+  </si>
+  <si>
+    <t>Problemas del empirismo lógico</t>
+  </si>
+  <si>
+    <t>Popper: contra el empirismo lógico</t>
+  </si>
+  <si>
+    <t>Kuhn: ciencia normal</t>
+  </si>
+  <si>
+    <t>Kuhn: ciencia revolucionaria</t>
+  </si>
+  <si>
+    <t>Ciencia y valores: la responsabilidad científica</t>
+  </si>
+  <si>
+    <t>(*) Fine, A. (1986). The Shaky Game.  Chicago, USA: The University of Chicago Press. Caps 1 y 3</t>
+  </si>
+  <si>
+    <t>(*) Fine, A. (1986). The Shaky Game.  Chicago, USA: The University of Chicago Press. Cap 5</t>
+  </si>
+  <si>
+    <t>Quine, W. V. O. (2002) Desde un punto de vista lógico. Paidos: Barcelona, España. Cap. 2</t>
+  </si>
+  <si>
+    <r>
+      <t>Popper, K (2002) </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>Conjeturas y refutaciones. Paidos: Barcelona, España. Cap 1 (★)</t>
+    </r>
   </si>
   <si>
     <r>
@@ -565,17 +507,95 @@
         <color theme="1"/>
         <rFont val="Inherit"/>
       </rPr>
-      <t>. Fondo de cultura económica: México.</t>
+      <t>. Fondo de cultura económica: México. Caps 1, 2,  3 y 4</t>
     </r>
   </si>
   <si>
-    <t>Ciencia y valores: Filosofía feminista de la ciencia</t>
-  </si>
-  <si>
-    <t>Ciencia y valores: la responsabilidad por el conocimiento</t>
-  </si>
-  <si>
-    <t>Harding, Ciencia y Feminismo (Cap 1),  Pinnich, The feminist approach to the philosophy of science</t>
+    <r>
+      <t>Kuhn, Thomas (1962) </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>La estructura de las revoluciones científicas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>. Fondo de cultura económica: México. Caps 5, 6, 7 y 8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Kuhn, Thomas (1962) </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>La estructura de las revoluciones científicas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>. Fondo de cultura económica: México. Caps 9, 10, 11 y 12</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Harding, Ciencia y Feminismo (Cap 1), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arrieta de Guzmán, Teresa (2018) Sobre el pensamiento feminista y la ciencia
+. En  </t>
+  </si>
+  <si>
+    <r>
+      <t>Douglas, Heather E. (2003). The Moral Responsibilities of Scientists (Tensions between Autonomy and Responsibility). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>American Philosophical Quarterly</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> 40 (1):59 - 68.</t>
+    </r>
+  </si>
+  <si>
+    <t>Taller final</t>
+  </si>
+  <si>
+    <t>Taller primer corte</t>
+  </si>
+  <si>
+    <t>Taller segundo corte</t>
+  </si>
+  <si>
+    <t>Taller tercer corte</t>
   </si>
 </sst>
 </file>
@@ -642,19 +662,6 @@
       <name val="Inherit"/>
     </font>
     <font>
-      <sz val="28"/>
-      <color rgb="FFEAEAEA"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="28"/>
-      <color rgb="FFEAEAEA"/>
-      <name val="PingFang SC"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -678,6 +685,19 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -795,9 +815,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -819,20 +839,20 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
@@ -840,54 +860,55 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency [0]" xfId="1" builtinId="7"/>
@@ -1237,8 +1258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{126E7679-38D8-C743-97BF-FED867349053}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C11" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1259,25 +1280,25 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>3</v>
@@ -1285,18 +1306,18 @@
     </row>
     <row r="2" spans="1:14" ht="34">
       <c r="A2" s="5">
-        <v>43850</v>
+        <v>44033</v>
       </c>
       <c r="B2" s="3" t="str">
         <f>PROPER(TEXT(A2,"[$-240a] dddd dd mmmm"))</f>
-        <v xml:space="preserve"> Lunes 20 Enero</v>
+        <v xml:space="preserve"> Martes 21 Julio</v>
       </c>
       <c r="C2" s="5">
-        <v>43854</v>
+        <v>44036</v>
       </c>
       <c r="D2" s="3" t="str">
         <f>PROPER(TEXT(C2,"[$-240a] dddd dd mmmm"))</f>
-        <v xml:space="preserve"> Viernes 24 Enero</v>
+        <v xml:space="preserve"> Viernes 24 Julio</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>4</v>
@@ -1306,7 +1327,7 @@
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -1315,28 +1336,28 @@
     </row>
     <row r="3" spans="1:14" ht="50" customHeight="1">
       <c r="A3" s="5">
-        <v>43857</v>
+        <v>44040</v>
       </c>
       <c r="B3" s="3" t="str">
         <f t="shared" ref="B3:B19" si="0">PROPER(TEXT(A3,"[$-240a] dddd dd mmmm"))</f>
-        <v xml:space="preserve"> Lunes 27 Enero</v>
+        <v xml:space="preserve"> Martes 28 Julio</v>
       </c>
       <c r="C3" s="5">
-        <v>43861</v>
+        <v>44043</v>
       </c>
       <c r="D3" s="3" t="str">
         <f t="shared" ref="D3:D19" si="1">PROPER(TEXT(C3,"[$-240a] dddd dd mmmm"))</f>
-        <v xml:space="preserve"> Viernes 31 Enero</v>
+        <v xml:space="preserve"> Viernes 31 Julio</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="9" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -1345,18 +1366,18 @@
     </row>
     <row r="4" spans="1:14" ht="50" customHeight="1">
       <c r="A4" s="5">
-        <v>43864</v>
+        <v>44047</v>
       </c>
       <c r="B4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Lunes 03 Febrero</v>
+        <v xml:space="preserve"> Martes 04 Agosto</v>
       </c>
       <c r="C4" s="5">
-        <v>43868</v>
+        <v>44050</v>
       </c>
       <c r="D4" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> Viernes 07 Febrero</v>
+        <v xml:space="preserve"> Viernes 07 Agosto</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>6</v>
@@ -1366,7 +1387,7 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="9" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -1375,27 +1396,27 @@
     </row>
     <row r="5" spans="1:14" ht="50" customHeight="1">
       <c r="A5" s="5">
-        <v>43871</v>
+        <v>44054</v>
       </c>
       <c r="B5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Lunes 10 Febrero</v>
+        <v xml:space="preserve"> Martes 11 Agosto</v>
       </c>
       <c r="C5" s="5">
-        <v>43875</v>
+        <v>44057</v>
       </c>
       <c r="D5" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> Viernes 14 Febrero</v>
+        <v xml:space="preserve"> Viernes 14 Agosto</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>28</v>
+        <v>115</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -1404,24 +1425,27 @@
     </row>
     <row r="6" spans="1:14" ht="74" customHeight="1">
       <c r="A6" s="5">
-        <v>43878</v>
+        <v>44061</v>
       </c>
       <c r="B6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Lunes 17 Febrero</v>
+        <v xml:space="preserve"> Martes 18 Agosto</v>
       </c>
       <c r="C6" s="5">
-        <v>43882</v>
+        <v>44064</v>
       </c>
       <c r="D6" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> Viernes 21 Febrero</v>
+        <v xml:space="preserve"> Viernes 21 Agosto</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>122</v>
+        <v>105</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -1430,30 +1454,30 @@
     </row>
     <row r="7" spans="1:14" ht="50" customHeight="1">
       <c r="A7" s="5">
-        <v>43885</v>
+        <v>44068</v>
       </c>
       <c r="B7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Lunes 24 Febrero</v>
+        <v xml:space="preserve"> Martes 25 Agosto</v>
       </c>
       <c r="C7" s="5">
-        <v>43889</v>
+        <v>44071</v>
       </c>
       <c r="D7" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> Viernes 28 Febrero</v>
+        <v xml:space="preserve"> Viernes 28 Agosto</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H7" t="s">
         <v>21</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="H7" t="s">
-        <v>29</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -1464,28 +1488,28 @@
     </row>
     <row r="8" spans="1:14" ht="50" customHeight="1">
       <c r="A8" s="5">
-        <v>43892</v>
+        <v>44075</v>
       </c>
       <c r="B8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Lunes 02 Marzo</v>
+        <v xml:space="preserve"> Martes 01 Septiembre</v>
       </c>
       <c r="C8" s="5">
-        <v>43896</v>
+        <v>44078</v>
       </c>
       <c r="D8" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> Viernes 06 Marzo</v>
+        <v xml:space="preserve"> Viernes 04 Septiembre</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>22</v>
+        <v>109</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>22</v>
+        <v>109</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -1494,28 +1518,28 @@
     </row>
     <row r="9" spans="1:14" ht="50" customHeight="1">
       <c r="A9" s="5">
-        <v>43899</v>
+        <v>44082</v>
       </c>
       <c r="B9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Lunes 09 Marzo</v>
+        <v xml:space="preserve"> Martes 08 Septiembre</v>
       </c>
       <c r="C9" s="5">
-        <v>43903</v>
+        <v>44085</v>
       </c>
       <c r="D9" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> Viernes 13 Marzo</v>
+        <v xml:space="preserve"> Viernes 11 Septiembre</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>22</v>
+        <v>109</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>22</v>
+        <v>109</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1524,28 +1548,28 @@
     </row>
     <row r="10" spans="1:14" ht="50" customHeight="1">
       <c r="A10" s="5">
-        <v>43906</v>
+        <v>44089</v>
       </c>
       <c r="B10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Lunes 16 Marzo</v>
+        <v xml:space="preserve"> Martes 15 Septiembre</v>
       </c>
       <c r="C10" s="5">
-        <v>43910</v>
+        <v>44092</v>
       </c>
       <c r="D10" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> Viernes 20 Marzo</v>
+        <v xml:space="preserve"> Viernes 18 Septiembre</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" t="s">
-        <v>30</v>
+        <v>117</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -1554,28 +1578,28 @@
     </row>
     <row r="11" spans="1:14" ht="50" customHeight="1">
       <c r="A11" s="5">
-        <v>43913</v>
+        <v>44096</v>
       </c>
       <c r="B11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Lunes 23 Marzo</v>
+        <v xml:space="preserve"> Martes 22 Septiembre</v>
       </c>
       <c r="C11" s="5">
-        <v>43917</v>
+        <v>44099</v>
       </c>
       <c r="D11" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> Viernes 27 Marzo</v>
+        <v xml:space="preserve"> Viernes 25 Septiembre</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>12</v>
+        <v>111</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="10" t="s">
-        <v>31</v>
+        <v>118</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -1584,30 +1608,30 @@
     </row>
     <row r="12" spans="1:14" ht="50" customHeight="1">
       <c r="A12" s="5">
-        <v>43920</v>
+        <v>44103</v>
       </c>
       <c r="B12" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Lunes 30 Marzo</v>
+        <v xml:space="preserve"> Martes 29 Septiembre</v>
       </c>
       <c r="C12" s="5">
-        <v>43924</v>
+        <v>44106</v>
       </c>
       <c r="D12" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> Viernes 03 Abril</v>
+        <v xml:space="preserve"> Viernes 02 Octubre</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>20</v>
+        <v>112</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>32</v>
+        <v>119</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1616,26 +1640,29 @@
     </row>
     <row r="13" spans="1:14" ht="99" customHeight="1">
       <c r="A13" s="5">
-        <v>43927</v>
+        <v>44110</v>
       </c>
       <c r="B13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Lunes 06 Abril</v>
+        <v xml:space="preserve"> Martes 06 Octubre</v>
       </c>
       <c r="C13" s="5">
-        <v>43931</v>
+        <v>44113</v>
       </c>
       <c r="D13" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> Viernes 10 Abril</v>
+        <v xml:space="preserve"> Viernes 09 Octubre</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>14</v>
+        <v>112</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>14</v>
+        <v>112</v>
       </c>
       <c r="G13" s="1"/>
+      <c r="H13" s="10" t="s">
+        <v>120</v>
+      </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1643,27 +1670,29 @@
     </row>
     <row r="14" spans="1:14" ht="50" customHeight="1">
       <c r="A14" s="5">
-        <v>43934</v>
+        <v>44117</v>
       </c>
       <c r="B14" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Lunes 13 Abril</v>
+        <v xml:space="preserve"> Martes 13 Octubre</v>
       </c>
       <c r="C14" s="5">
-        <v>43938</v>
+        <v>44120</v>
       </c>
       <c r="D14" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> Viernes 17 Abril</v>
+        <v xml:space="preserve"> Viernes 16 Octubre</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="G14" s="1"/>
-      <c r="H14" s="10"/>
+      <c r="H14" s="10" t="s">
+        <v>121</v>
+      </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1671,26 +1700,29 @@
     </row>
     <row r="15" spans="1:14" ht="50" customHeight="1">
       <c r="A15" s="5">
-        <v>43941</v>
+        <v>44124</v>
       </c>
       <c r="B15" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Lunes 20 Abril</v>
+        <v xml:space="preserve"> Martes 20 Octubre</v>
       </c>
       <c r="C15" s="5">
-        <v>43945</v>
+        <v>44127</v>
       </c>
       <c r="D15" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> Viernes 24 Abril</v>
+        <v xml:space="preserve"> Viernes 23 Octubre</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="G15" s="1"/>
+      <c r="H15" s="37" t="s">
+        <v>122</v>
+      </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -1698,28 +1730,28 @@
     </row>
     <row r="16" spans="1:14" ht="50" customHeight="1">
       <c r="A16" s="5">
-        <v>43948</v>
+        <v>44131</v>
       </c>
       <c r="B16" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Lunes 27 Abril</v>
+        <v xml:space="preserve"> Martes 27 Octubre</v>
       </c>
       <c r="C16" s="5">
-        <v>43952</v>
+        <v>44134</v>
       </c>
       <c r="D16" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> Viernes 01 Mayo</v>
+        <v xml:space="preserve"> Viernes 30 Octubre</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>19</v>
+        <v>107</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>20</v>
+        <v>107</v>
       </c>
       <c r="G16" s="2"/>
-      <c r="H16" s="10" t="s">
-        <v>125</v>
+      <c r="H16" s="37" t="s">
+        <v>123</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -1728,28 +1760,28 @@
     </row>
     <row r="17" spans="1:12" ht="50" customHeight="1">
       <c r="A17" s="5">
-        <v>43955</v>
+        <v>44138</v>
       </c>
       <c r="B17" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Lunes 04 Mayo</v>
+        <v xml:space="preserve"> Martes 03 Noviembre</v>
       </c>
       <c r="C17" s="5">
-        <v>43959</v>
+        <v>44141</v>
       </c>
       <c r="D17" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> Viernes 08 Mayo</v>
+        <v xml:space="preserve"> Viernes 06 Noviembre</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="G17" s="2"/>
-      <c r="H17" s="37" t="s">
-        <v>128</v>
+      <c r="H17" s="38" t="s">
+        <v>124</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -1758,59 +1790,45 @@
     </row>
     <row r="18" spans="1:12" ht="50" customHeight="1">
       <c r="A18" s="5">
-        <v>43962</v>
+        <v>44145</v>
       </c>
       <c r="B18" s="3" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Lunes 11 Mayo</v>
+        <v xml:space="preserve"> Martes 10 Noviembre</v>
       </c>
       <c r="C18" s="5">
-        <v>43966</v>
+        <v>44148</v>
       </c>
       <c r="D18" s="3" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> Viernes 15 Mayo</v>
+        <v xml:space="preserve"> Viernes 13 Noviembre</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>127</v>
+        <v>9</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="10"/>
+        <v>125</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>98</v>
+      </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" ht="50" customHeight="1">
-      <c r="A19" s="5">
-        <v>43969</v>
-      </c>
-      <c r="B19" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> Lunes 18 Mayo</v>
-      </c>
-      <c r="C19" s="5">
-        <v>43973</v>
-      </c>
-      <c r="D19" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> Viernes 22 Mayo</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>109</v>
-      </c>
+      <c r="A19" s="5"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -1839,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{908C0474-4D48-F842-927C-22B5DB315036}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:J24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1860,67 +1878,67 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="L1" s="2"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="20" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G2" s="21"/>
       <c r="H2" s="20" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J2" s="8"/>
       <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="16" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
@@ -1943,7 +1961,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="16" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B4" s="17"/>
       <c r="C4" s="17"/>
@@ -1966,7 +1984,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="16" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -1989,7 +2007,7 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="16" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -2012,7 +2030,7 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="16" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -2035,7 +2053,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="16" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2058,7 +2076,7 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="16" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -2081,7 +2099,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="16" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -2104,7 +2122,7 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="16" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
@@ -2127,7 +2145,7 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="16" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
@@ -2150,7 +2168,7 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="16" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
@@ -2173,7 +2191,7 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="16" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
@@ -2196,7 +2214,7 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="16" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
@@ -2219,7 +2237,7 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="16" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
@@ -2242,7 +2260,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="16" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -2265,7 +2283,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="16" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -2339,12 +2357,12 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="22" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
       <c r="D1" s="23" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E1" s="23"/>
       <c r="F1" s="23"/>
@@ -2363,12 +2381,12 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="22" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
       <c r="D2" s="23" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="E2" s="23"/>
       <c r="F2" s="23"/>
@@ -2387,16 +2405,16 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="22" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B3" s="22"/>
       <c r="C3" s="22" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
       <c r="F3" s="22" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="G3" s="22"/>
       <c r="H3" s="22"/>
@@ -2413,16 +2431,16 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="24" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B4" s="24"/>
       <c r="C4" s="22" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>
       <c r="F4" s="22" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="G4" s="22"/>
       <c r="H4" s="22"/>
@@ -2439,16 +2457,16 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="24" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B5" s="24"/>
       <c r="C5" s="22" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
       <c r="F5" s="22" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="G5" s="22"/>
       <c r="H5" s="22"/>
@@ -2465,16 +2483,16 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" s="25" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B6" s="25"/>
       <c r="C6" s="25" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D6" s="25"/>
       <c r="E6" s="25"/>
       <c r="F6" s="25" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="G6" s="25"/>
       <c r="H6" s="25"/>
@@ -2491,67 +2509,67 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" s="15" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="C7" s="27"/>
       <c r="D7" s="28"/>
       <c r="E7" s="29" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="F7" s="30"/>
       <c r="G7" s="15" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="K7" s="15" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="L7" s="15" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="M7" s="15" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="N7" s="26" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="O7" s="28"/>
       <c r="P7" s="15" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="Q7" s="15" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="R7" s="15" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="14" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C8" s="32"/>
       <c r="D8" s="33"/>
       <c r="E8" s="31" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="F8" s="33"/>
       <c r="G8" s="14" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
@@ -2563,25 +2581,25 @@
       <c r="O8" s="35"/>
       <c r="P8" s="12"/>
       <c r="Q8" s="13" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="R8" s="12"/>
     </row>
     <row r="9" spans="1:18">
       <c r="A9" s="14" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="33"/>
       <c r="E9" s="31" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="F9" s="33"/>
       <c r="G9" s="14" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
@@ -2593,25 +2611,25 @@
       <c r="O9" s="35"/>
       <c r="P9" s="12"/>
       <c r="Q9" s="13" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="R9" s="12"/>
     </row>
     <row r="10" spans="1:18">
       <c r="A10" s="14" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="C10" s="32"/>
       <c r="D10" s="33"/>
       <c r="E10" s="31" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="F10" s="33"/>
       <c r="G10" s="14" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
@@ -2623,25 +2641,25 @@
       <c r="O10" s="35"/>
       <c r="P10" s="12"/>
       <c r="Q10" s="13" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="R10" s="12"/>
     </row>
     <row r="11" spans="1:18">
       <c r="A11" s="14" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C11" s="32"/>
       <c r="D11" s="33"/>
       <c r="E11" s="31" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="F11" s="33"/>
       <c r="G11" s="14" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
@@ -2653,25 +2671,25 @@
       <c r="O11" s="35"/>
       <c r="P11" s="12"/>
       <c r="Q11" s="13" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="R11" s="12"/>
     </row>
     <row r="12" spans="1:18">
       <c r="A12" s="14" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="C12" s="32"/>
       <c r="D12" s="33"/>
       <c r="E12" s="31" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="F12" s="33"/>
       <c r="G12" s="14" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
@@ -2683,25 +2701,25 @@
       <c r="O12" s="35"/>
       <c r="P12" s="12"/>
       <c r="Q12" s="13" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="R12" s="12"/>
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="14" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C13" s="32"/>
       <c r="D13" s="33"/>
       <c r="E13" s="31" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="F13" s="33"/>
       <c r="G13" s="14" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
@@ -2713,25 +2731,25 @@
       <c r="O13" s="35"/>
       <c r="P13" s="12"/>
       <c r="Q13" s="13" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="R13" s="12"/>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="14" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C14" s="32"/>
       <c r="D14" s="33"/>
       <c r="E14" s="31" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="F14" s="33"/>
       <c r="G14" s="14" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
@@ -2743,25 +2761,25 @@
       <c r="O14" s="35"/>
       <c r="P14" s="12"/>
       <c r="Q14" s="13" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="R14" s="12"/>
     </row>
     <row r="15" spans="1:18">
       <c r="A15" s="14" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C15" s="32"/>
       <c r="D15" s="33"/>
       <c r="E15" s="31" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="F15" s="33"/>
       <c r="G15" s="14" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
@@ -2773,25 +2791,25 @@
       <c r="O15" s="35"/>
       <c r="P15" s="12"/>
       <c r="Q15" s="13" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="R15" s="12"/>
     </row>
     <row r="16" spans="1:18">
       <c r="A16" s="14" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C16" s="32"/>
       <c r="D16" s="33"/>
       <c r="E16" s="31" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="F16" s="33"/>
       <c r="G16" s="14" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
@@ -2803,25 +2821,25 @@
       <c r="O16" s="35"/>
       <c r="P16" s="12"/>
       <c r="Q16" s="13" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="R16" s="12"/>
     </row>
     <row r="17" spans="1:18">
       <c r="A17" s="14" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C17" s="32"/>
       <c r="D17" s="33"/>
       <c r="E17" s="31" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="F17" s="33"/>
       <c r="G17" s="14" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
@@ -2833,25 +2851,25 @@
       <c r="O17" s="35"/>
       <c r="P17" s="12"/>
       <c r="Q17" s="13" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="R17" s="12"/>
     </row>
     <row r="18" spans="1:18">
       <c r="A18" s="14" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="C18" s="32"/>
       <c r="D18" s="33"/>
       <c r="E18" s="31" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F18" s="33"/>
       <c r="G18" s="14" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
@@ -2863,25 +2881,25 @@
       <c r="O18" s="35"/>
       <c r="P18" s="12"/>
       <c r="Q18" s="13" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="R18" s="12"/>
     </row>
     <row r="19" spans="1:18">
       <c r="A19" s="14" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C19" s="32"/>
       <c r="D19" s="33"/>
       <c r="E19" s="31" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="F19" s="33"/>
       <c r="G19" s="14" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
@@ -2893,25 +2911,25 @@
       <c r="O19" s="35"/>
       <c r="P19" s="12"/>
       <c r="Q19" s="13" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="R19" s="12"/>
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="14" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C20" s="32"/>
       <c r="D20" s="33"/>
       <c r="E20" s="31" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="F20" s="33"/>
       <c r="G20" s="14" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
@@ -2923,25 +2941,25 @@
       <c r="O20" s="35"/>
       <c r="P20" s="12"/>
       <c r="Q20" s="13" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="R20" s="12"/>
     </row>
     <row r="21" spans="1:18">
       <c r="A21" s="14" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C21" s="32"/>
       <c r="D21" s="33"/>
       <c r="E21" s="31" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="F21" s="33"/>
       <c r="G21" s="14" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
@@ -2953,25 +2971,25 @@
       <c r="O21" s="35"/>
       <c r="P21" s="12"/>
       <c r="Q21" s="13" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="R21" s="12"/>
     </row>
     <row r="22" spans="1:18">
       <c r="A22" s="14" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C22" s="32"/>
       <c r="D22" s="33"/>
       <c r="E22" s="31" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="F22" s="33"/>
       <c r="G22" s="14" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
@@ -2983,25 +3001,25 @@
       <c r="O22" s="35"/>
       <c r="P22" s="12"/>
       <c r="Q22" s="13" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="R22" s="12"/>
     </row>
     <row r="23" spans="1:18">
       <c r="A23" s="14" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C23" s="32"/>
       <c r="D23" s="33"/>
       <c r="E23" s="31" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="F23" s="33"/>
       <c r="G23" s="14" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
@@ -3013,13 +3031,13 @@
       <c r="O23" s="35"/>
       <c r="P23" s="12"/>
       <c r="Q23" s="13" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="R23" s="12"/>
     </row>
     <row r="24" spans="1:18">
       <c r="A24" s="36" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B24" s="36"/>
       <c r="C24" s="36"/>

</xml_diff>

<commit_message>
filo feminista de la ciencia
</commit_message>
<xml_diff>
--- a/HFC.xlsx
+++ b/HFC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JCES\Documents\GitHub\filociencia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CAD615B-40D6-4A3F-9455-C908059F8467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C48C15B-A815-4498-A1B6-D38339CD5AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{92AD9A07-1A21-864F-8FD9-98EB9AF3C646}"/>
+    <workbookView xWindow="6120" yWindow="2040" windowWidth="18720" windowHeight="11385" xr2:uid="{92AD9A07-1A21-864F-8FD9-98EB9AF3C646}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="129">
   <si>
     <t>Mtext</t>
   </si>
@@ -451,9 +451,6 @@
     <t>Kuhn: ciencia revolucionaria</t>
   </si>
   <si>
-    <t>Ciencia y valores: la responsabilidad científica</t>
-  </si>
-  <si>
     <t>(*) Fine, A. (1986). The Shaky Game.  Chicago, USA: The University of Chicago Press. Caps 1 y 3</t>
   </si>
   <si>
@@ -594,6 +591,12 @@
   <si>
     <t>Miércoles</t>
   </si>
+  <si>
+    <t>festivo</t>
+  </si>
+  <si>
+    <t>Tema por definir</t>
+  </si>
 </sst>
 </file>
 
@@ -604,9 +607,16 @@
     <numFmt numFmtId="165" formatCode="[$-240A]dddd\ d&quot; de &quot;mmmm&quot; de &quot;yyyy;@"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -696,6 +706,14 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -811,10 +829,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -825,7 +843,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -834,22 +852,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
@@ -857,55 +875,59 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda [0]" xfId="1" builtinId="7"/>
@@ -1255,8 +1277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{126E7679-38D8-C743-97BF-FED867349053}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="G13" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -1289,10 +1311,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>126</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>127</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>96</v>
@@ -1407,13 +1429,13 @@
         <v xml:space="preserve"> Viernes 14 Agosto</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -1442,7 +1464,7 @@
         <v>102</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -1566,7 +1588,7 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -1596,7 +1618,7 @@
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -1628,7 +1650,7 @@
         <v>101</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1658,7 +1680,7 @@
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -1688,7 +1710,7 @@
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1711,14 +1733,14 @@
         <v xml:space="preserve"> Viernes 23 Octubre</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>104</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -1747,10 +1769,10 @@
         <v>104</v>
       </c>
       <c r="G16" s="2"/>
-      <c r="H16" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="I16" s="1"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="39" t="s">
+        <v>118</v>
+      </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1771,14 +1793,14 @@
         <v xml:space="preserve"> Viernes 06 Noviembre</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -1804,10 +1826,10 @@
         <v>8</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H18" s="10" t="s">
         <v>97</v>
@@ -1847,6 +1869,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1878,7 +1901,7 @@
         <v>21</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>90</v>
@@ -1887,7 +1910,7 @@
         <v>23</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>91</v>
@@ -1896,7 +1919,7 @@
         <v>94</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>92</v>

</xml_diff>